<commit_message>
them redu, undu, fix solve.
</commit_message>
<xml_diff>
--- a/bkh.xlsx
+++ b/bkh.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieun\Desktop\GitHub\sudoku\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Tìm hiểu về các stack</t>
   </si>
@@ -119,13 +114,16 @@
     <t>Trước dự kiến( 04/10/2018)</t>
   </si>
   <si>
-    <t>Trể hẹn</t>
+    <t>Trể hẹn( Hoàn thành 20/10/2018)</t>
+  </si>
+  <si>
+    <t>Hoàn tthành(09/10/2018)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -447,7 +445,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -482,7 +480,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -659,7 +657,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,7 +668,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +678,7 @@
     <col min="3" max="3" width="17.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="1" customWidth="1"/>
     <col min="5" max="6" width="24.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -825,7 +823,9 @@
       <c r="F7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">

</xml_diff>